<commit_message>
some bullshit, please stop
</commit_message>
<xml_diff>
--- a/usanew/usa2016_try2/new_york/ny_levels.xlsx
+++ b/usanew/usa2016_try2/new_york/ny_levels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="520" windowWidth="18700" windowHeight="15580" tabRatio="500"/>
+    <workbookView xWindow="9020" yWindow="680" windowWidth="18700" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
   <si>
     <t>SUMLEV</t>
   </si>
@@ -225,16 +225,38 @@
   </si>
   <si>
     <t>Yonkers city</t>
+  </si>
+  <si>
+    <t>Mamaroneck village</t>
+  </si>
+  <si>
+    <t>Briarcliff Manor village</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,13 +279,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,9 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29:S29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -966,7 +998,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>157</v>
+        <v>71</v>
       </c>
       <c r="B8">
         <v>36</v>
@@ -978,13 +1010,13 @@
         <v>48890</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>48895</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
@@ -2111,37 +2143,46 @@
         <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="J27" t="s">
         <v>21</v>
       </c>
       <c r="K27">
-        <v>11315</v>
+        <f>K46+K47</f>
+        <v>18929</v>
       </c>
       <c r="L27">
-        <v>11315</v>
+        <f t="shared" ref="L27:S27" si="0">L46+L47</f>
+        <v>18930</v>
       </c>
       <c r="M27">
-        <v>11330</v>
+        <f t="shared" si="0"/>
+        <v>18954</v>
       </c>
       <c r="N27">
-        <v>11398</v>
+        <f t="shared" si="0"/>
+        <v>19066</v>
       </c>
       <c r="O27">
-        <v>11418</v>
+        <f t="shared" si="0"/>
+        <v>19101</v>
       </c>
       <c r="P27">
-        <v>11490</v>
+        <f t="shared" si="0"/>
+        <v>19224</v>
       </c>
       <c r="Q27">
-        <v>11511</v>
+        <f t="shared" si="0"/>
+        <v>19258</v>
       </c>
       <c r="R27">
-        <v>11543</v>
+        <f t="shared" si="0"/>
+        <v>19306</v>
       </c>
       <c r="S27">
-        <v>11574</v>
+        <f t="shared" si="0"/>
+        <v>19356</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -2204,62 +2245,50 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>71</v>
-      </c>
-      <c r="B29">
-        <v>36</v>
-      </c>
-      <c r="C29">
-        <v>119</v>
-      </c>
-      <c r="D29">
-        <v>8103</v>
-      </c>
-      <c r="E29">
-        <v>49011</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
       <c r="H29" t="s">
         <v>19</v>
       </c>
       <c r="I29" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="J29" t="s">
         <v>21</v>
       </c>
       <c r="K29">
-        <v>659</v>
+        <f>K48+K49</f>
+        <v>7867</v>
       </c>
       <c r="L29">
-        <v>659</v>
+        <f t="shared" ref="L29:S29" si="1">L48+L49</f>
+        <v>7836</v>
       </c>
       <c r="M29">
-        <v>660</v>
+        <f t="shared" si="1"/>
+        <v>7840</v>
       </c>
       <c r="N29">
-        <v>666</v>
+        <f t="shared" si="1"/>
+        <v>7914</v>
       </c>
       <c r="O29">
-        <v>668</v>
+        <f t="shared" si="1"/>
+        <v>7918</v>
       </c>
       <c r="P29">
-        <v>677</v>
+        <f t="shared" si="1"/>
+        <v>7938</v>
       </c>
       <c r="Q29">
-        <v>679</v>
+        <f t="shared" si="1"/>
+        <v>7978</v>
       </c>
       <c r="R29">
-        <v>682</v>
+        <f t="shared" si="1"/>
+        <v>8020</v>
       </c>
       <c r="S29">
-        <v>683</v>
+        <f t="shared" si="1"/>
+        <v>8032</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
@@ -2568,7 +2597,7 @@
         <v>119</v>
       </c>
       <c r="D35">
-        <v>8103</v>
+        <v>55530</v>
       </c>
       <c r="E35">
         <v>55541</v>
@@ -2583,37 +2612,37 @@
         <v>19</v>
       </c>
       <c r="I35" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J35" t="s">
         <v>21</v>
       </c>
       <c r="K35">
-        <v>7208</v>
+        <v>25060</v>
       </c>
       <c r="L35">
-        <v>7177</v>
+        <v>25069</v>
       </c>
       <c r="M35">
-        <v>7180</v>
+        <v>25068</v>
       </c>
       <c r="N35">
-        <v>7248</v>
+        <v>25239</v>
       </c>
       <c r="O35">
-        <v>7250</v>
+        <v>25188</v>
       </c>
       <c r="P35">
-        <v>7261</v>
+        <v>25261</v>
       </c>
       <c r="Q35">
-        <v>7299</v>
+        <v>25328</v>
       </c>
       <c r="R35">
-        <v>7338</v>
+        <v>25369</v>
       </c>
       <c r="S35">
-        <v>7349</v>
+        <v>25360</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
@@ -2627,7 +2656,7 @@
         <v>119</v>
       </c>
       <c r="D36">
-        <v>55530</v>
+        <v>99990</v>
       </c>
       <c r="E36">
         <v>55541</v>
@@ -2639,40 +2668,40 @@
         <v>1</v>
       </c>
       <c r="H36" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J36" t="s">
         <v>21</v>
       </c>
       <c r="K36">
-        <v>25060</v>
+        <v>5406</v>
       </c>
       <c r="L36">
-        <v>25069</v>
+        <v>5428</v>
       </c>
       <c r="M36">
-        <v>25068</v>
+        <v>5437</v>
       </c>
       <c r="N36">
-        <v>25239</v>
+        <v>5475</v>
       </c>
       <c r="O36">
-        <v>25188</v>
+        <v>5497</v>
       </c>
       <c r="P36">
-        <v>25261</v>
+        <v>5529</v>
       </c>
       <c r="Q36">
-        <v>25328</v>
+        <v>5541</v>
       </c>
       <c r="R36">
-        <v>25369</v>
+        <v>5581</v>
       </c>
       <c r="S36">
-        <v>25360</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
@@ -2686,10 +2715,10 @@
         <v>119</v>
       </c>
       <c r="D37">
-        <v>99990</v>
+        <v>57001</v>
       </c>
       <c r="E37">
-        <v>55541</v>
+        <v>57012</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2698,40 +2727,40 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J37" t="s">
         <v>21</v>
       </c>
       <c r="K37">
-        <v>5406</v>
+        <v>6910</v>
       </c>
       <c r="L37">
-        <v>5428</v>
+        <v>6910</v>
       </c>
       <c r="M37">
-        <v>5437</v>
+        <v>6917</v>
       </c>
       <c r="N37">
-        <v>5475</v>
+        <v>6955</v>
       </c>
       <c r="O37">
-        <v>5497</v>
+        <v>6964</v>
       </c>
       <c r="P37">
-        <v>5529</v>
+        <v>7001</v>
       </c>
       <c r="Q37">
-        <v>5541</v>
+        <v>7011</v>
       </c>
       <c r="R37">
-        <v>5581</v>
+        <v>7022</v>
       </c>
       <c r="S37">
-        <v>5594</v>
+        <v>7020</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -2745,7 +2774,7 @@
         <v>119</v>
       </c>
       <c r="D38">
-        <v>57001</v>
+        <v>57023</v>
       </c>
       <c r="E38">
         <v>57012</v>
@@ -2760,37 +2789,37 @@
         <v>19</v>
       </c>
       <c r="I38" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J38" t="s">
         <v>21</v>
       </c>
       <c r="K38">
-        <v>6910</v>
+        <v>5486</v>
       </c>
       <c r="L38">
-        <v>6910</v>
+        <v>5486</v>
       </c>
       <c r="M38">
-        <v>6917</v>
+        <v>5493</v>
       </c>
       <c r="N38">
-        <v>6955</v>
+        <v>5529</v>
       </c>
       <c r="O38">
-        <v>6964</v>
+        <v>5535</v>
       </c>
       <c r="P38">
-        <v>7001</v>
+        <v>5565</v>
       </c>
       <c r="Q38">
-        <v>7011</v>
+        <v>5571</v>
       </c>
       <c r="R38">
-        <v>7022</v>
+        <v>5573</v>
       </c>
       <c r="S38">
-        <v>7020</v>
+        <v>5565</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
@@ -2804,10 +2833,10 @@
         <v>119</v>
       </c>
       <c r="D39">
-        <v>57023</v>
+        <v>64309</v>
       </c>
       <c r="E39">
-        <v>57012</v>
+        <v>64309</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2819,37 +2848,37 @@
         <v>19</v>
       </c>
       <c r="I39" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J39" t="s">
         <v>21</v>
       </c>
       <c r="K39">
-        <v>5486</v>
+        <v>15720</v>
       </c>
       <c r="L39">
-        <v>5486</v>
+        <v>15720</v>
       </c>
       <c r="M39">
-        <v>5493</v>
+        <v>15739</v>
       </c>
       <c r="N39">
-        <v>5529</v>
+        <v>15830</v>
       </c>
       <c r="O39">
-        <v>5535</v>
+        <v>15856</v>
       </c>
       <c r="P39">
-        <v>5565</v>
+        <v>15947</v>
       </c>
       <c r="Q39">
-        <v>5571</v>
+        <v>15970</v>
       </c>
       <c r="R39">
-        <v>5573</v>
+        <v>15990</v>
       </c>
       <c r="S39">
-        <v>5565</v>
+        <v>15980</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -2863,10 +2892,10 @@
         <v>119</v>
       </c>
       <c r="D40">
-        <v>64309</v>
+        <v>59223</v>
       </c>
       <c r="E40">
-        <v>64309</v>
+        <v>64320</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2878,37 +2907,37 @@
         <v>19</v>
       </c>
       <c r="I40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J40" t="s">
         <v>21</v>
       </c>
       <c r="K40">
-        <v>15720</v>
+        <v>28967</v>
       </c>
       <c r="L40">
-        <v>15720</v>
+        <v>28946</v>
       </c>
       <c r="M40">
-        <v>15739</v>
+        <v>28980</v>
       </c>
       <c r="N40">
-        <v>15830</v>
+        <v>29157</v>
       </c>
       <c r="O40">
-        <v>15856</v>
+        <v>29207</v>
       </c>
       <c r="P40">
-        <v>15947</v>
+        <v>29380</v>
       </c>
       <c r="Q40">
-        <v>15970</v>
+        <v>29443</v>
       </c>
       <c r="R40">
-        <v>15990</v>
+        <v>29503</v>
       </c>
       <c r="S40">
-        <v>15980</v>
+        <v>29524</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -2922,7 +2951,7 @@
         <v>119</v>
       </c>
       <c r="D41">
-        <v>44831</v>
+        <v>64325</v>
       </c>
       <c r="E41">
         <v>64320</v>
@@ -2937,37 +2966,37 @@
         <v>19</v>
       </c>
       <c r="I41" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="J41" t="s">
         <v>21</v>
       </c>
       <c r="K41">
-        <v>7614</v>
+        <v>9347</v>
       </c>
       <c r="L41">
-        <v>7615</v>
+        <v>9347</v>
       </c>
       <c r="M41">
-        <v>7624</v>
+        <v>9378</v>
       </c>
       <c r="N41">
-        <v>7668</v>
+        <v>9419</v>
       </c>
       <c r="O41">
-        <v>7683</v>
+        <v>9443</v>
       </c>
       <c r="P41">
-        <v>7734</v>
+        <v>9493</v>
       </c>
       <c r="Q41">
-        <v>7747</v>
+        <v>9519</v>
       </c>
       <c r="R41">
-        <v>7763</v>
+        <v>9558</v>
       </c>
       <c r="S41">
-        <v>7782</v>
+        <v>9575</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -2981,10 +3010,10 @@
         <v>119</v>
       </c>
       <c r="D42">
-        <v>59223</v>
+        <v>65431</v>
       </c>
       <c r="E42">
-        <v>64320</v>
+        <v>65442</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2996,37 +3025,37 @@
         <v>19</v>
       </c>
       <c r="I42" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J42" t="s">
         <v>21</v>
       </c>
       <c r="K42">
-        <v>28967</v>
+        <v>17166</v>
       </c>
       <c r="L42">
-        <v>28946</v>
+        <v>17166</v>
       </c>
       <c r="M42">
-        <v>28980</v>
+        <v>17195</v>
       </c>
       <c r="N42">
-        <v>29157</v>
+        <v>17342</v>
       </c>
       <c r="O42">
-        <v>29207</v>
+        <v>17455</v>
       </c>
       <c r="P42">
-        <v>29380</v>
+        <v>17596</v>
       </c>
       <c r="Q42">
-        <v>29443</v>
+        <v>17694</v>
       </c>
       <c r="R42">
-        <v>29503</v>
+        <v>17819</v>
       </c>
       <c r="S42">
-        <v>29524</v>
+        <v>17909</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
@@ -3040,10 +3069,10 @@
         <v>119</v>
       </c>
       <c r="D43">
-        <v>64325</v>
+        <v>81677</v>
       </c>
       <c r="E43">
-        <v>64320</v>
+        <v>81677</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -3055,37 +3084,37 @@
         <v>19</v>
       </c>
       <c r="I43" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J43" t="s">
         <v>21</v>
       </c>
       <c r="K43">
-        <v>9347</v>
+        <v>56853</v>
       </c>
       <c r="L43">
-        <v>9347</v>
+        <v>56853</v>
       </c>
       <c r="M43">
-        <v>9378</v>
+        <v>56942</v>
       </c>
       <c r="N43">
-        <v>9419</v>
+        <v>57227</v>
       </c>
       <c r="O43">
-        <v>9443</v>
+        <v>57338</v>
       </c>
       <c r="P43">
-        <v>9493</v>
+        <v>57812</v>
       </c>
       <c r="Q43">
-        <v>9519</v>
+        <v>57920</v>
       </c>
       <c r="R43">
-        <v>9558</v>
+        <v>58248</v>
       </c>
       <c r="S43">
-        <v>9575</v>
+        <v>58241</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -3099,10 +3128,10 @@
         <v>119</v>
       </c>
       <c r="D44">
-        <v>65431</v>
+        <v>84000</v>
       </c>
       <c r="E44">
-        <v>65442</v>
+        <v>84000</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -3114,96 +3143,37 @@
         <v>19</v>
       </c>
       <c r="I44" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J44" t="s">
         <v>21</v>
       </c>
       <c r="K44">
-        <v>17166</v>
+        <v>195976</v>
       </c>
       <c r="L44">
-        <v>17166</v>
+        <v>195979</v>
       </c>
       <c r="M44">
-        <v>17195</v>
+        <v>196386</v>
       </c>
       <c r="N44">
-        <v>17342</v>
+        <v>197720</v>
       </c>
       <c r="O44">
-        <v>17455</v>
+        <v>198290</v>
       </c>
       <c r="P44">
-        <v>17596</v>
+        <v>199266</v>
       </c>
       <c r="Q44">
-        <v>17694</v>
+        <v>199932</v>
       </c>
       <c r="R44">
-        <v>17819</v>
+        <v>200367</v>
       </c>
       <c r="S44">
-        <v>17909</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>71</v>
-      </c>
-      <c r="B45">
-        <v>36</v>
-      </c>
-      <c r="C45">
-        <v>119</v>
-      </c>
-      <c r="D45">
-        <v>81677</v>
-      </c>
-      <c r="E45">
-        <v>81677</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
-        <v>19</v>
-      </c>
-      <c r="I45" t="s">
-        <v>64</v>
-      </c>
-      <c r="J45" t="s">
-        <v>21</v>
-      </c>
-      <c r="K45">
-        <v>56853</v>
-      </c>
-      <c r="L45">
-        <v>56853</v>
-      </c>
-      <c r="M45">
-        <v>56942</v>
-      </c>
-      <c r="N45">
-        <v>57227</v>
-      </c>
-      <c r="O45">
-        <v>57338</v>
-      </c>
-      <c r="P45">
-        <v>57812</v>
-      </c>
-      <c r="Q45">
-        <v>57920</v>
-      </c>
-      <c r="R45">
-        <v>58248</v>
-      </c>
-      <c r="S45">
-        <v>58241</v>
+        <v>200807</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -3217,10 +3187,10 @@
         <v>119</v>
       </c>
       <c r="D46">
-        <v>84000</v>
+        <v>44831</v>
       </c>
       <c r="E46">
-        <v>84000</v>
+        <v>44842</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -3232,37 +3202,214 @@
         <v>19</v>
       </c>
       <c r="I46" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="J46" t="s">
         <v>21</v>
       </c>
       <c r="K46">
-        <v>195976</v>
+        <v>11315</v>
       </c>
       <c r="L46">
-        <v>195979</v>
+        <v>11315</v>
       </c>
       <c r="M46">
-        <v>196386</v>
+        <v>11330</v>
       </c>
       <c r="N46">
-        <v>197720</v>
+        <v>11398</v>
       </c>
       <c r="O46">
-        <v>198290</v>
+        <v>11418</v>
       </c>
       <c r="P46">
-        <v>199266</v>
+        <v>11490</v>
       </c>
       <c r="Q46">
-        <v>199932</v>
+        <v>11511</v>
       </c>
       <c r="R46">
-        <v>200367</v>
+        <v>11543</v>
       </c>
       <c r="S46">
-        <v>200807</v>
+        <v>11574</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>71</v>
+      </c>
+      <c r="B47">
+        <v>36</v>
+      </c>
+      <c r="C47">
+        <v>119</v>
+      </c>
+      <c r="D47">
+        <v>44831</v>
+      </c>
+      <c r="E47">
+        <v>64320</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" t="s">
+        <v>46</v>
+      </c>
+      <c r="J47" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47">
+        <v>7614</v>
+      </c>
+      <c r="L47">
+        <v>7615</v>
+      </c>
+      <c r="M47">
+        <v>7624</v>
+      </c>
+      <c r="N47">
+        <v>7668</v>
+      </c>
+      <c r="O47">
+        <v>7683</v>
+      </c>
+      <c r="P47">
+        <v>7734</v>
+      </c>
+      <c r="Q47">
+        <v>7747</v>
+      </c>
+      <c r="R47">
+        <v>7763</v>
+      </c>
+      <c r="S47">
+        <v>7782</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>71</v>
+      </c>
+      <c r="B48">
+        <v>36</v>
+      </c>
+      <c r="C48">
+        <v>119</v>
+      </c>
+      <c r="D48">
+        <v>8103</v>
+      </c>
+      <c r="E48">
+        <v>49011</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" t="s">
+        <v>49</v>
+      </c>
+      <c r="J48" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48">
+        <v>659</v>
+      </c>
+      <c r="L48">
+        <v>659</v>
+      </c>
+      <c r="M48">
+        <v>660</v>
+      </c>
+      <c r="N48">
+        <v>666</v>
+      </c>
+      <c r="O48">
+        <v>668</v>
+      </c>
+      <c r="P48">
+        <v>677</v>
+      </c>
+      <c r="Q48">
+        <v>679</v>
+      </c>
+      <c r="R48">
+        <v>682</v>
+      </c>
+      <c r="S48">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>71</v>
+      </c>
+      <c r="B49">
+        <v>36</v>
+      </c>
+      <c r="C49">
+        <v>119</v>
+      </c>
+      <c r="D49">
+        <v>8103</v>
+      </c>
+      <c r="E49">
+        <v>55541</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>49</v>
+      </c>
+      <c r="J49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K49">
+        <v>7208</v>
+      </c>
+      <c r="L49">
+        <v>7177</v>
+      </c>
+      <c r="M49">
+        <v>7180</v>
+      </c>
+      <c r="N49">
+        <v>7248</v>
+      </c>
+      <c r="O49">
+        <v>7250</v>
+      </c>
+      <c r="P49">
+        <v>7261</v>
+      </c>
+      <c r="Q49">
+        <v>7299</v>
+      </c>
+      <c r="R49">
+        <v>7338</v>
+      </c>
+      <c r="S49">
+        <v>7349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>